<commit_message>
add AE, SUPPAE, LB and SUPPLB
</commit_message>
<xml_diff>
--- a/TDF_CS_ReleaseNotes.xlsx
+++ b/TDF_CS_ReleaseNotes.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -17,12 +17,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Details!$A$1:$M$67</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="171">
   <si>
     <t>Pinnacle 21 ID</t>
   </si>
@@ -289,6 +289,252 @@
   </si>
   <si>
     <t>QLABEL, 9</t>
+  </si>
+  <si>
+    <t>CT2002</t>
+  </si>
+  <si>
+    <t>FDAC341</t>
+  </si>
+  <si>
+    <t>CT2003</t>
+  </si>
+  <si>
+    <t>FDAC342</t>
+  </si>
+  <si>
+    <t>Consistency</t>
+  </si>
+  <si>
+    <t>SD0021</t>
+  </si>
+  <si>
+    <t>FDAC117</t>
+  </si>
+  <si>
+    <t>Missing End Time-Point value</t>
+  </si>
+  <si>
+    <t>SD1090</t>
+  </si>
+  <si>
+    <t>FDAC131</t>
+  </si>
+  <si>
+    <t>SD1201</t>
+  </si>
+  <si>
+    <t>FDAC213</t>
+  </si>
+  <si>
+    <t>AE</t>
+  </si>
+  <si>
+    <t>AEDTC</t>
+  </si>
+  <si>
+    <t>EPOCH, AE</t>
+  </si>
+  <si>
+    <t>AEDY</t>
+  </si>
+  <si>
+    <t>Missing AEDY variable, when AEDTC variable is present</t>
+  </si>
+  <si>
+    <t>AEENDTC</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>SUB:RFSTDTC, AESTDTC, AESTDY</t>
+  </si>
+  <si>
+    <t>2013-05-09, 2013-05-09, 366</t>
+  </si>
+  <si>
+    <t>Incorrect value for AESTDY variable</t>
+  </si>
+  <si>
+    <t>AEDECOD, AETERM, AESEV, AESTDTC, USUBJID</t>
+  </si>
+  <si>
+    <t>ERYTHEMA, ERYTHEMA, MILD, 2012-08-07, 01-701-1023</t>
+  </si>
+  <si>
+    <t>Duplicate records in AE domain</t>
+  </si>
+  <si>
+    <t>LB</t>
+  </si>
+  <si>
+    <t>EPOCH, LB</t>
+  </si>
+  <si>
+    <t>LBORRESU</t>
+  </si>
+  <si>
+    <t>MILL/uL</t>
+  </si>
+  <si>
+    <t>LBORRESU value not found in 'Unit' extensible codelist</t>
+  </si>
+  <si>
+    <t>NO UNITS</t>
+  </si>
+  <si>
+    <t>THOU/uL</t>
+  </si>
+  <si>
+    <t>pg/mL</t>
+  </si>
+  <si>
+    <t>uIU/mL</t>
+  </si>
+  <si>
+    <t>LBSTRESU</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>LBSTRESU value not found in 'Unit' extensible codelist</t>
+  </si>
+  <si>
+    <t>GI/L</t>
+  </si>
+  <si>
+    <t>TI/L</t>
+  </si>
+  <si>
+    <t>fmol(Fe)</t>
+  </si>
+  <si>
+    <t>LBTEST</t>
+  </si>
+  <si>
+    <t>Blood Urea Nitrogen</t>
+  </si>
+  <si>
+    <t>LBTEST value not found in 'Laboratory Test Name' extensible codelist</t>
+  </si>
+  <si>
+    <t>Platelet</t>
+  </si>
+  <si>
+    <t>LBTESTCD</t>
+  </si>
+  <si>
+    <t>BUN</t>
+  </si>
+  <si>
+    <t>LBTESTCD value not found in 'Laboratory Test Code' extensible codelist</t>
+  </si>
+  <si>
+    <t>LBTESTCD, LBTEST</t>
+  </si>
+  <si>
+    <t>PLAT, Platelet</t>
+  </si>
+  <si>
+    <t>LBTESTCD and LBTEST values do not have the same Code in CDISC CT</t>
+  </si>
+  <si>
+    <t>SUPPAE</t>
+  </si>
+  <si>
+    <t>QEVAL, 178</t>
+  </si>
+  <si>
+    <t>QVAL, 199</t>
+  </si>
+  <si>
+    <t>IDVARVAL, 198</t>
+  </si>
+  <si>
+    <t>QORIG, 193</t>
+  </si>
+  <si>
+    <t>QLABEL, 17</t>
+  </si>
+  <si>
+    <t>SUPPLB</t>
+  </si>
+  <si>
+    <t>IDVARVAL</t>
+  </si>
+  <si>
+    <t>Unexpected character value in IDVARVAL variable</t>
+  </si>
+  <si>
+    <t>[6 spaces]63</t>
+  </si>
+  <si>
+    <t>QVAL, 197</t>
+  </si>
+  <si>
+    <t>IDVARVAL, 192</t>
+  </si>
+  <si>
+    <t>QLABEL, 8</t>
+  </si>
+  <si>
+    <t>Many of these - no change necessary</t>
+  </si>
+  <si>
+    <t>add AEDY</t>
+  </si>
+  <si>
+    <t>add EPOCH</t>
+  </si>
+  <si>
+    <t>added EPOCH</t>
+  </si>
+  <si>
+    <t>added AEDY</t>
+  </si>
+  <si>
+    <t>correct value</t>
+  </si>
+  <si>
+    <t>recalculated based on RFSTDTC and AESTDTD</t>
+  </si>
+  <si>
+    <t>change to 10^12/L</t>
+  </si>
+  <si>
+    <t>remove words "NO UNIT" and leave missing</t>
+  </si>
+  <si>
+    <t>change to 10^9/L</t>
+  </si>
+  <si>
+    <t>change to ng/L</t>
+  </si>
+  <si>
+    <t>change to mIU/L</t>
+  </si>
+  <si>
+    <t>remove value of 1 from LBSTRESU</t>
+  </si>
+  <si>
+    <t>change to fmol</t>
+  </si>
+  <si>
+    <t>change to UREAN</t>
+  </si>
+  <si>
+    <t>change to Urea Nitrogen</t>
+  </si>
+  <si>
+    <t>change to Platelets</t>
+  </si>
+  <si>
+    <t>fixed by changing Platelet to Platelets</t>
+  </si>
+  <si>
+    <t>Many of these - trim(left(idvarval))</t>
   </si>
 </sst>
 </file>
@@ -697,13 +943,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M80"/>
+  <dimension ref="A1:M114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F70" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B107" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K75" sqref="K75:M80"/>
+      <selection pane="bottomRight" activeCell="A114" sqref="A114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3767,6 +4013,1235 @@
         <v>79</v>
       </c>
     </row>
+    <row r="81" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G81" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J81" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K81" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G82" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J82" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K82" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="L82" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="M82" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G83" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I83" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J83" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K83" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="L83" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="M83" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B84" s="1">
+        <v>1</v>
+      </c>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="G84" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I84" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J84" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K84" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B85" s="1">
+        <v>971</v>
+      </c>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G85" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I85" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J85" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K85" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="L85" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="M85" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B86" s="1">
+        <v>7</v>
+      </c>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G86" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I86" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J86" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K86" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G87" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I87" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J87" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K87" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L87" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="M87" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I88" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J88" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K88" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L88" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="M88" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I89" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J89" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K89" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L89" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="M89" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
+      <c r="D90" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I90" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J90" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K90" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L90" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="M90" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I91" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J91" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K91" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L91" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="M91" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I92" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J92" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K92" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L92" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="M92" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I93" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J93" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K93" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L93" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="M93" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G94" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I94" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J94" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K94" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L94" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="M94" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B95" s="1"/>
+      <c r="C95" s="1">
+        <v>1809</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F95" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G95" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I95" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J95" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K95" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="M95" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B96" s="1"/>
+      <c r="C96" s="1">
+        <v>4663</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I96" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J96" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K96" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="M96" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B97" s="1"/>
+      <c r="C97" s="1">
+        <v>10829</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I97" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J97" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K97" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="M97" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B98" s="1"/>
+      <c r="C98" s="1">
+        <v>272</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I98" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J98" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K98" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="M98" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B99" s="1"/>
+      <c r="C99" s="1">
+        <v>271</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I99" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J99" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K99" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="M99" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B100" s="1"/>
+      <c r="C100" s="1">
+        <v>1798</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F100" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G100" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H100" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I100" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J100" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K100" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="M100" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B101" s="1"/>
+      <c r="C101" s="1">
+        <v>10829</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H101" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I101" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J101" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K101" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="M101" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A102" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B102" s="1"/>
+      <c r="C102" s="1">
+        <v>1809</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H102" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I102" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J102" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K102" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="M102" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B103" s="1"/>
+      <c r="C103" s="1">
+        <v>1809</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I103" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J103" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K103" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="M103" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A104" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B104" s="1"/>
+      <c r="C104" s="1">
+        <v>1828</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F104" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G104" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I104" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J104" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K104" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="M104" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B105" s="1"/>
+      <c r="C105" s="1">
+        <v>1788</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I105" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J105" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K105" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="M105" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A106" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B106" s="1"/>
+      <c r="C106" s="1">
+        <v>1828</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F106" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G106" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="I106" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J106" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K106" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="M106" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A107" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B107" s="1"/>
+      <c r="C107" s="1">
+        <v>1788</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F107" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="G107" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I107" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J107" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K107" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="M107" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A108" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B108" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="I108" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J108" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K108" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+      <c r="A109" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B109" s="1"/>
+      <c r="C109" s="1"/>
+      <c r="D109" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F109" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G109" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I109" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J109" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K109" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L109" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="M109" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+      <c r="A110" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B110" s="1"/>
+      <c r="C110" s="1"/>
+      <c r="D110" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I110" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J110" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K110" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L110" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="M110" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+      <c r="A111" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B111" s="1"/>
+      <c r="C111" s="1"/>
+      <c r="D111" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I111" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J111" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K111" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L111" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="M111" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+      <c r="A112" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B112" s="1"/>
+      <c r="C112" s="1"/>
+      <c r="D112" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H112" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I112" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J112" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K112" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L112" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="M112" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+      <c r="A113" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B113" s="1"/>
+      <c r="C113" s="1"/>
+      <c r="D113" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I113" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J113" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K113" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L113" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="M113" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+      <c r="A114" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B114" s="1"/>
+      <c r="C114" s="1"/>
+      <c r="D114" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I114" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J114" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K114" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L114" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="M114" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" location="'Rules'!A158" display="SD1076"/>
@@ -3789,8 +5264,138 @@
     <hyperlink ref="G73" location="'Rules'!A159" display="FDAC021"/>
     <hyperlink ref="F74" location="'Rules'!A162" display="SD1082"/>
     <hyperlink ref="G74" location="'Rules'!A162" display="FDAC036"/>
-    <hyperlink ref="F75" location="'Rules'!A162" display="SD1082"/>
-    <hyperlink ref="G75" location="'Rules'!A162" display="FDAC036"/>
+    <hyperlink ref="F75" location="'Rules'!A186" display="SD1108"/>
+    <hyperlink ref="G75" location="'Rules'!A186" display="FDAC007"/>
+    <hyperlink ref="F76" location="'Rules'!A187" display="SD1109"/>
+    <hyperlink ref="G76" location="'Rules'!A187" display="FDAC004"/>
+    <hyperlink ref="F77" location="'Rules'!A188" display="SD1110"/>
+    <hyperlink ref="G77" location="'Rules'!A188" display="FDAC003"/>
+    <hyperlink ref="F78" location="'Rules'!A162" display="SD1082"/>
+    <hyperlink ref="G78" location="'Rules'!A162" display="FDAC036"/>
+    <hyperlink ref="F79" location="'Rules'!A191" display="SD1113"/>
+    <hyperlink ref="G79" location="'Rules'!A191" display="FDAC010"/>
+    <hyperlink ref="F80" location="'Rules'!A194" display="SD1115"/>
+    <hyperlink ref="G80" location="'Rules'!A194" display="FDAC002"/>
+    <hyperlink ref="F81" location="'Rules'!A13" display="SD0006"/>
+    <hyperlink ref="G81" location="'Rules'!A13" display="FDAC113"/>
+    <hyperlink ref="F82" location="'Rules'!A286" display="SD2236"/>
+    <hyperlink ref="G82" location="'Rules'!A286" display="FDAC197"/>
+    <hyperlink ref="F83" location="'Rules'!A163" display="SD1083"/>
+    <hyperlink ref="G83" location="'Rules'!A163" display="FDAC124"/>
+    <hyperlink ref="F84" location="'Rules'!A28" display="SD0021"/>
+    <hyperlink ref="G84" location="'Rules'!A28" display="FDAC117"/>
+    <hyperlink ref="F557" location="'Rules'!A162" display="SD1082"/>
+    <hyperlink ref="G557" location="'Rules'!A162" display="FDAC036"/>
+    <hyperlink ref="F564" location="'Rules'!A170" display="SD1090"/>
+    <hyperlink ref="G564" location="'Rules'!A170" display="FDAC131"/>
+    <hyperlink ref="F565" location="'Rules'!A210" display="SD1201"/>
+    <hyperlink ref="G565" location="'Rules'!A210" display="FDAC213"/>
+    <hyperlink ref="F795" location="'Rules'!A13" display="SD0006"/>
+    <hyperlink ref="G795" location="'Rules'!A13" display="FDAC113"/>
+    <hyperlink ref="F796" location="'Rules'!A286" display="SD2236"/>
+    <hyperlink ref="G796" location="'Rules'!A286" display="FDAC197"/>
+    <hyperlink ref="F808" location="'Rules'!A159" display="SD1077"/>
+    <hyperlink ref="G808" location="'Rules'!A159" display="FDAC021"/>
+    <hyperlink ref="F809" location="'Rules'!A3" display="CT2002"/>
+    <hyperlink ref="G809" location="'Rules'!A3" display="FDAC341"/>
+    <hyperlink ref="F814" location="'Rules'!A3" display="CT2002"/>
+    <hyperlink ref="G814" location="'Rules'!A3" display="FDAC341"/>
+    <hyperlink ref="F818" location="'Rules'!A3" display="CT2002"/>
+    <hyperlink ref="G818" location="'Rules'!A3" display="FDAC341"/>
+    <hyperlink ref="F820" location="'Rules'!A3" display="CT2002"/>
+    <hyperlink ref="G820" location="'Rules'!A3" display="FDAC341"/>
+    <hyperlink ref="F821" location="'Rules'!A4" display="CT2003"/>
+    <hyperlink ref="G821" location="'Rules'!A4" display="FDAC342"/>
+    <hyperlink ref="F822" location="'Rules'!A36" display="SD0029"/>
+    <hyperlink ref="G822" location="'Rules'!A36" display="FDAC169"/>
+    <hyperlink ref="F1140" location="'Rules'!A162" display="SD1082"/>
+    <hyperlink ref="G1140" location="'Rules'!A162" display="FDAC036"/>
+    <hyperlink ref="F1143" location="'Rules'!A158" display="SD1076"/>
+    <hyperlink ref="G1143" location="'Rules'!A158" display="FDAC031"/>
+    <hyperlink ref="F1145" location="'Rules'!A162" display="SD1082"/>
+    <hyperlink ref="G1145" location="'Rules'!A162" display="FDAC036"/>
+    <hyperlink ref="F1152" location="'Rules'!A81" display="SD0077"/>
+    <hyperlink ref="G1152" location="'Rules'!A81" display="FDAC074"/>
+    <hyperlink ref="F2152" location="'Rules'!A113" display="SD1021"/>
+    <hyperlink ref="G2152" location="'Rules'!A113" display="FDAC216"/>
+    <hyperlink ref="F3152" location="'Rules'!A162" display="SD1082"/>
+    <hyperlink ref="G3152" location="'Rules'!A162" display="FDAC036"/>
+    <hyperlink ref="F3158" location="'Rules'!A158" display="SD1076"/>
+    <hyperlink ref="G3158" location="'Rules'!A158" display="FDAC031"/>
+    <hyperlink ref="F85" location="'Rules'!A158" display="SD1076"/>
+    <hyperlink ref="G85" location="'Rules'!A158" display="FDAC031"/>
+    <hyperlink ref="F86" location="'Rules'!A210" display="SD1201"/>
+    <hyperlink ref="G86" location="'Rules'!A210" display="FDAC213"/>
+    <hyperlink ref="F316" location="'Rules'!A13" display="SD0006"/>
+    <hyperlink ref="G316" location="'Rules'!A13" display="FDAC113"/>
+    <hyperlink ref="F317" location="'Rules'!A286" display="SD2236"/>
+    <hyperlink ref="G317" location="'Rules'!A286" display="FDAC197"/>
+    <hyperlink ref="F329" location="'Rules'!A159" display="SD1077"/>
+    <hyperlink ref="G329" location="'Rules'!A159" display="FDAC021"/>
+    <hyperlink ref="F330" location="'Rules'!A3" display="CT2002"/>
+    <hyperlink ref="G330" location="'Rules'!A3" display="FDAC341"/>
+    <hyperlink ref="F335" location="'Rules'!A3" display="CT2002"/>
+    <hyperlink ref="G335" location="'Rules'!A3" display="FDAC341"/>
+    <hyperlink ref="F339" location="'Rules'!A3" display="CT2002"/>
+    <hyperlink ref="G339" location="'Rules'!A3" display="FDAC341"/>
+    <hyperlink ref="F341" location="'Rules'!A3" display="CT2002"/>
+    <hyperlink ref="G341" location="'Rules'!A3" display="FDAC341"/>
+    <hyperlink ref="F342" location="'Rules'!A4" display="CT2003"/>
+    <hyperlink ref="G342" location="'Rules'!A4" display="FDAC342"/>
+    <hyperlink ref="F343" location="'Rules'!A36" display="SD0029"/>
+    <hyperlink ref="G343" location="'Rules'!A36" display="FDAC169"/>
+    <hyperlink ref="F661" location="'Rules'!A162" display="SD1082"/>
+    <hyperlink ref="G661" location="'Rules'!A162" display="FDAC036"/>
+    <hyperlink ref="F664" location="'Rules'!A158" display="SD1076"/>
+    <hyperlink ref="G664" location="'Rules'!A158" display="FDAC031"/>
+    <hyperlink ref="F666" location="'Rules'!A162" display="SD1082"/>
+    <hyperlink ref="G666" location="'Rules'!A162" display="FDAC036"/>
+    <hyperlink ref="F673" location="'Rules'!A81" display="SD0077"/>
+    <hyperlink ref="G673" location="'Rules'!A81" display="FDAC074"/>
+    <hyperlink ref="F1673" location="'Rules'!A113" display="SD1021"/>
+    <hyperlink ref="G1673" location="'Rules'!A113" display="FDAC216"/>
+    <hyperlink ref="F2673" location="'Rules'!A162" display="SD1082"/>
+    <hyperlink ref="G2673" location="'Rules'!A162" display="FDAC036"/>
+    <hyperlink ref="F2679" location="'Rules'!A158" display="SD1076"/>
+    <hyperlink ref="G2679" location="'Rules'!A158" display="FDAC031"/>
+    <hyperlink ref="F87" location="'Rules'!A162" display="SD1082"/>
+    <hyperlink ref="G87" location="'Rules'!A162" display="FDAC036"/>
+    <hyperlink ref="F1094" location="'Rules'!A113" display="SD1021"/>
+    <hyperlink ref="G1094" location="'Rules'!A113" display="FDAC216"/>
+    <hyperlink ref="F2094" location="'Rules'!A162" display="SD1082"/>
+    <hyperlink ref="G2094" location="'Rules'!A162" display="FDAC036"/>
+    <hyperlink ref="F2100" location="'Rules'!A158" display="SD1076"/>
+    <hyperlink ref="G2100" location="'Rules'!A158" display="FDAC031"/>
+    <hyperlink ref="F94" location="'Rules'!A159" display="SD1077"/>
+    <hyperlink ref="G94" location="'Rules'!A159" display="FDAC021"/>
+    <hyperlink ref="F95" location="'Rules'!A3" display="CT2002"/>
+    <hyperlink ref="G95" location="'Rules'!A3" display="FDAC341"/>
+    <hyperlink ref="F100" location="'Rules'!A3" display="CT2002"/>
+    <hyperlink ref="G100" location="'Rules'!A3" display="FDAC341"/>
+    <hyperlink ref="F104" location="'Rules'!A3" display="CT2002"/>
+    <hyperlink ref="G104" location="'Rules'!A3" display="FDAC341"/>
+    <hyperlink ref="F106" location="'Rules'!A3" display="CT2002"/>
+    <hyperlink ref="G106" location="'Rules'!A3" display="FDAC341"/>
+    <hyperlink ref="F107" location="'Rules'!A4" display="CT2003"/>
+    <hyperlink ref="G107" location="'Rules'!A4" display="FDAC342"/>
+    <hyperlink ref="F426" location="'Rules'!A162" display="SD1082"/>
+    <hyperlink ref="G426" location="'Rules'!A162" display="FDAC036"/>
+    <hyperlink ref="F429" location="'Rules'!A158" display="SD1076"/>
+    <hyperlink ref="G429" location="'Rules'!A158" display="FDAC031"/>
+    <hyperlink ref="F431" location="'Rules'!A162" display="SD1082"/>
+    <hyperlink ref="G431" location="'Rules'!A162" display="FDAC036"/>
+    <hyperlink ref="F438" location="'Rules'!A81" display="SD0077"/>
+    <hyperlink ref="G438" location="'Rules'!A81" display="FDAC074"/>
+    <hyperlink ref="F1438" location="'Rules'!A113" display="SD1021"/>
+    <hyperlink ref="G1438" location="'Rules'!A113" display="FDAC216"/>
+    <hyperlink ref="F2438" location="'Rules'!A162" display="SD1082"/>
+    <hyperlink ref="G2438" location="'Rules'!A162" display="FDAC036"/>
+    <hyperlink ref="F2444" location="'Rules'!A158" display="SD1076"/>
+    <hyperlink ref="G2444" location="'Rules'!A158" display="FDAC031"/>
+    <hyperlink ref="F109" location="'Rules'!A162" display="SD1082"/>
+    <hyperlink ref="G109" location="'Rules'!A162" display="FDAC036"/>
+    <hyperlink ref="F115" location="'Rules'!A158" display="SD1076"/>
+    <hyperlink ref="G115" location="'Rules'!A158" display="FDAC031"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>